<commit_message>
till 30 min done
</commit_message>
<xml_diff>
--- a/fo high low.xlsx
+++ b/fo high low.xlsx
@@ -451,7 +451,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>814.1</v>
+        <v>797.6</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>797.75</v>
+        <v>773.6</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>785.6</v>
+        <v>787</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>805.65</v>
+        <v>790.35</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>148</v>
+        <v>192</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>800.75</v>
+        <v>786.7</v>
       </c>
     </row>
     <row r="3">
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>878</v>
+        <v>889.6</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>860.5</v>
+        <v>856.15</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>873.15</v>
+        <v>876</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>867.85</v>
+        <v>875.5</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>874.35</v>
+        <v>860.7</v>
       </c>
     </row>
     <row r="4">
@@ -550,22 +550,22 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>44720</v>
+        <v>44347.55</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>44392.4</v>
+        <v>43982.4</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>44124.4</v>
+        <v>44219.7</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>44464.35</v>
+        <v>44234.05</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>44531.9</v>
+        <v>44025</v>
       </c>
     </row>
     <row r="5">
@@ -575,22 +575,22 @@
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>340.55</v>
+        <v>332.7</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>331.2</v>
+        <v>323.65</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>326.6</v>
+        <v>329.55</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>333.9</v>
+        <v>330.8</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>123</v>
+        <v>192</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>332.1</v>
+        <v>327.5</v>
       </c>
     </row>
     <row r="6">
@@ -600,22 +600,22 @@
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>494.5</v>
+        <v>474.8</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>482.35</v>
+        <v>464.8</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>469.5</v>
+        <v>472</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>484.35</v>
+        <v>472.95</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>493.5</v>
+        <v>471.4</v>
       </c>
     </row>
     <row r="7">
@@ -625,22 +625,22 @@
         </is>
       </c>
       <c r="B7" s="1" t="n">
-        <v>463.35</v>
+        <v>454.6</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>458.15</v>
+        <v>448.6</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>451.7</v>
+        <v>451.1</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>460.6</v>
+        <v>451.6</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>463</v>
+        <v>449.85</v>
       </c>
     </row>
     <row r="8">
@@ -650,22 +650,22 @@
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>963.9</v>
+        <v>964.15</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>954.7</v>
+        <v>951.45</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>957.65</v>
+        <v>960.9</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>958</v>
+        <v>961.2</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>960.4</v>
+        <v>953.2</v>
       </c>
     </row>
     <row r="9">
@@ -675,22 +675,22 @@
         </is>
       </c>
       <c r="B9" s="1" t="n">
-        <v>702</v>
+        <v>680.45</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>665.95</v>
+        <v>657.3</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>665.95</v>
+        <v>662</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>699.1</v>
+        <v>662.4</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>668.15</v>
+        <v>677.7</v>
       </c>
     </row>
     <row r="10">
@@ -700,22 +700,22 @@
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>19552.8</v>
+        <v>19506.25</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>19488.6</v>
+        <v>19316.85</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>19399.85</v>
+        <v>19471.2</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>19504.35</v>
+        <v>19478.35</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>19532.05</v>
+        <v>19334.15</v>
       </c>
     </row>
     <row r="11">
@@ -725,22 +725,22 @@
         </is>
       </c>
       <c r="B11" s="1" t="n">
-        <v>2563.45</v>
+        <v>2581.75</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>2518</v>
+        <v>2527.8</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>2562.55</v>
+        <v>2576</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>2551.45</v>
+        <v>2577.45</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>2532</v>
+        <v>2529.7</v>
       </c>
     </row>
     <row r="12">
@@ -750,22 +750,22 @@
         </is>
       </c>
       <c r="B12" s="1" t="n">
-        <v>582</v>
+        <v>567.1</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>574.1</v>
+        <v>560.75</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>561.85</v>
+        <v>563</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>576.75</v>
+        <v>563.2</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>204</v>
+        <v>314</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>575.25</v>
+        <v>565.9</v>
       </c>
     </row>
     <row r="13">
@@ -775,22 +775,22 @@
         </is>
       </c>
       <c r="B13" s="1" t="n">
-        <v>848.65</v>
+        <v>847.1</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>838.1</v>
+        <v>832.6</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>837.55</v>
+        <v>846.5</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>839.3</v>
+        <v>845.95</v>
       </c>
       <c r="F13" s="1" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>847</v>
+        <v>832.85</v>
       </c>
     </row>
     <row r="14">
@@ -800,22 +800,22 @@
         </is>
       </c>
       <c r="B14" s="1" t="n">
-        <v>627.1</v>
+        <v>610.15</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>613.55</v>
+        <v>596.25</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>603.95</v>
+        <v>607.95</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>614.5</v>
+        <v>608.25</v>
       </c>
       <c r="F14" s="1" t="n">
-        <v>131</v>
+        <v>196</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>623.85</v>
+        <v>598.55</v>
       </c>
     </row>
     <row r="15">
@@ -825,22 +825,22 @@
         </is>
       </c>
       <c r="B15" s="1" t="n">
-        <v>122.05</v>
+        <v>119.15</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>119.4</v>
+        <v>117.5</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>117.95</v>
+        <v>118.35</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>120.95</v>
+        <v>118.45</v>
       </c>
       <c r="F15" s="1" t="n">
-        <v>298</v>
+        <v>419</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>119.7</v>
+        <v>118.95</v>
       </c>
     </row>
     <row r="16">
@@ -850,22 +850,22 @@
         </is>
       </c>
       <c r="B16" s="1" t="n">
-        <v>3478.5</v>
+        <v>3461.45</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>3425</v>
+        <v>3423</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>3431.7</v>
+        <v>3458.4</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>3457.75</v>
+        <v>3457.45</v>
       </c>
       <c r="F16" s="1" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>3459.35</v>
+        <v>3438.25</v>
       </c>
     </row>
     <row r="17">
@@ -875,22 +875,22 @@
         </is>
       </c>
       <c r="B17" s="1" t="n">
-        <v>3073</v>
+        <v>3026.75</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>3000.6</v>
+        <v>2996.05</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>3012</v>
+        <v>3023</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>3026.9</v>
+        <v>3021.35</v>
       </c>
       <c r="F17" s="1" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>3009.05</v>
+        <v>3008.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DONE NEST AUTOMATION(VER 1)
</commit_message>
<xml_diff>
--- a/fo high low.xlsx
+++ b/fo high low.xlsx
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>845.3</v>
+        <v>828.75</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>820.7</v>
+        <v>806.75</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>826.9</v>
+        <v>821.4</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>823.7</v>
+        <v>821.95</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>832.05</v>
+        <v>807.9</v>
       </c>
     </row>
     <row r="3">
@@ -525,22 +525,22 @@
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>847</v>
+        <v>839.9</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>832.15</v>
+        <v>828</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>832.75</v>
+        <v>829</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>834.3</v>
+        <v>830.25</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>843.2</v>
+        <v>833.05</v>
       </c>
     </row>
     <row r="4">
@@ -550,22 +550,22 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>45009.95</v>
+        <v>44626</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>44525</v>
+        <v>44443.15</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>44525</v>
+        <v>44516.4</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>44559.1</v>
+        <v>44500.5</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>44817</v>
+        <v>44607</v>
       </c>
     </row>
     <row r="5">
@@ -575,22 +575,22 @@
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>337.85</v>
+        <v>328.65</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>331</v>
+        <v>325.5</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>331.9</v>
+        <v>327.2</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>332.5</v>
+        <v>327</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>336.65</v>
+        <v>328.65</v>
       </c>
     </row>
     <row r="6">
@@ -600,22 +600,22 @@
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>491.25</v>
+        <v>498.35</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>483.55</v>
+        <v>488.45</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>484.65</v>
+        <v>494.5</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>484.1</v>
+        <v>493.95</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>485.65</v>
+        <v>489.1</v>
       </c>
     </row>
     <row r="7">
@@ -625,22 +625,22 @@
         </is>
       </c>
       <c r="B7" s="1" t="n">
-        <v>464.75</v>
+        <v>459.15</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>454</v>
+        <v>448.5</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>456.15</v>
+        <v>457.35</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>456.1</v>
+        <v>456.55</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>464.5</v>
+        <v>450.1</v>
       </c>
     </row>
     <row r="8">
@@ -650,22 +650,22 @@
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>982.1</v>
+        <v>975.2</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>968.95</v>
+        <v>967</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>969.7</v>
+        <v>968.1</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>970.55</v>
+        <v>968.45</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>215</v>
+        <v>273</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>974.2</v>
+        <v>974.15</v>
       </c>
     </row>
     <row r="9">
@@ -675,22 +675,22 @@
         </is>
       </c>
       <c r="B9" s="1" t="n">
-        <v>667.35</v>
+        <v>679.9</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>647.65</v>
+        <v>657.75</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>648.15</v>
+        <v>675</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>649.6</v>
+        <v>675.35</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>129</v>
+        <v>90</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>664.25</v>
+        <v>660.6</v>
       </c>
     </row>
     <row r="10">
@@ -700,22 +700,22 @@
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>19575</v>
+        <v>19366.95</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>19376</v>
+        <v>19306</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>19390</v>
+        <v>19345.75</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>19395.6</v>
+        <v>19337.1</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>19543.4</v>
+        <v>19344.9</v>
       </c>
     </row>
     <row r="11">
@@ -725,22 +725,22 @@
         </is>
       </c>
       <c r="B11" s="1" t="n">
-        <v>2539.75</v>
+        <v>2442</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>2473</v>
+        <v>2410.5</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>2476</v>
+        <v>2423.15</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>2481</v>
+        <v>2422.45</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>2531.75</v>
+        <v>2433.05</v>
       </c>
     </row>
     <row r="12">
@@ -750,22 +750,22 @@
         </is>
       </c>
       <c r="B12" s="1" t="n">
-        <v>581.9</v>
+        <v>575.8</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>575.15</v>
+        <v>572</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>576.7</v>
+        <v>574.8</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>264</v>
+        <v>318</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>580.1</v>
+        <v>573.15</v>
       </c>
     </row>
     <row r="13">
@@ -775,22 +775,22 @@
         </is>
       </c>
       <c r="B13" s="1" t="n">
-        <v>854.65</v>
+        <v>841.5</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>843.55</v>
+        <v>834.75</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>845.8</v>
+        <v>836.8</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>844.75</v>
+        <v>836.6</v>
       </c>
       <c r="F13" s="1" t="n">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>848.9</v>
+        <v>838.9</v>
       </c>
     </row>
     <row r="14">
@@ -800,22 +800,22 @@
         </is>
       </c>
       <c r="B14" s="1" t="n">
-        <v>618.5</v>
+        <v>611.25</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>610.6</v>
+        <v>605.2</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>611.15</v>
+        <v>608.25</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>611.65</v>
+        <v>607.65</v>
       </c>
       <c r="F14" s="1" t="n">
-        <v>93</v>
+        <v>172</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>617.3</v>
+        <v>606.6</v>
       </c>
     </row>
     <row r="15">
@@ -825,22 +825,22 @@
         </is>
       </c>
       <c r="B15" s="1" t="n">
-        <v>120.3</v>
+        <v>120.35</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>118.05</v>
+        <v>117.8</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>118.25</v>
+        <v>120</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>118.25</v>
+        <v>119.7</v>
       </c>
       <c r="F15" s="1" t="n">
-        <v>336</v>
+        <v>950</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>119.9</v>
+        <v>118.2</v>
       </c>
     </row>
     <row r="16">
@@ -850,22 +850,22 @@
         </is>
       </c>
       <c r="B16" s="1" t="n">
-        <v>3415.5</v>
+        <v>3384.7</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>3380.95</v>
+        <v>3362.25</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>3389.95</v>
+        <v>3370.15</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>3386.25</v>
+        <v>3370.55</v>
       </c>
       <c r="F16" s="1" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>3410.2</v>
+        <v>3379.2</v>
       </c>
     </row>
     <row r="17">
@@ -875,22 +875,22 @@
         </is>
       </c>
       <c r="B17" s="1" t="n">
-        <v>3098.4</v>
+        <v>3086.45</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>3062.2</v>
+        <v>3046.05</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>3067.95</v>
+        <v>3075.4</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>3066.7</v>
+        <v>3074.7</v>
       </c>
       <c r="F17" s="1" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>3089.45</v>
+        <v>3050.55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>